<commit_message>
add more rows to situational dashboard
</commit_message>
<xml_diff>
--- a/SituationalDashboard.xlsx
+++ b/SituationalDashboard.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chart_index" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>data_level</t>
   </si>
@@ -159,6 +159,21 @@
     <t>District</t>
   </si>
   <si>
+    <t>Number of reported Non Polio AFP cases</t>
+  </si>
+  <si>
+    <t>Number of Unvaccinated Non Polio AFP Cases</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 1-3 doses</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 4-6 doses</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 7+ doses</t>
+  </si>
+  <si>
     <t>Number of inaccesible children</t>
   </si>
   <si>
@@ -205,7 +220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -246,6 +261,12 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,7 +290,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -280,6 +301,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -561,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -575,19 +597,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -898,15 +920,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="85.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.6640625" customWidth="1"/>
@@ -920,28 +941,28 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -949,16 +970,16 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
@@ -967,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>20</v>
@@ -978,13 +999,27 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="B3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -992,13 +1027,27 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1006,13 +1055,27 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1020,13 +1083,27 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1034,13 +1111,27 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1048,8 +1139,7 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -1062,8 +1152,7 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -1076,8 +1165,7 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1090,8 +1178,7 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -1104,8 +1191,7 @@
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>

</xml_diff>

<commit_message>
got dps working for 5 charts
</commit_message>
<xml_diff>
--- a/SituationalDashboard.xlsx
+++ b/SituationalDashboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="1360" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="2300" yWindow="4740" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="chart_index" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="142">
   <si>
     <t>t2</t>
     <phoneticPr fontId="9" type="noConversion"/>
@@ -31,6 +31,10 @@
   </si>
   <si>
     <t>Number of children missed due to all access issues</t>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>District</t>
@@ -857,8 +861,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
@@ -871,62 +875,62 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1">
         <v>28</v>
@@ -934,22 +938,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1">
         <v>28</v>
@@ -957,22 +961,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G5" s="1">
         <v>28</v>
@@ -980,22 +984,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="1">
         <v>16</v>
@@ -1003,22 +1007,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G7" s="1">
         <v>3</v>
@@ -1026,22 +1030,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G8" s="1">
         <v>28</v>
@@ -1049,22 +1053,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G9" s="1">
         <v>3</v>
@@ -1072,22 +1076,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
@@ -1095,22 +1099,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1118,22 +1122,22 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G12" s="1">
         <v>3</v>
@@ -1141,22 +1145,22 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G13" s="1">
         <v>3</v>
@@ -1164,28 +1168,29 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G14" s="1">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1201,8 +1206,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H15" sqref="A15:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
@@ -1222,28 +1227,28 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1251,16 +1256,16 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -1269,10 +1274,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1280,16 +1285,16 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -1298,10 +1303,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1310,16 +1315,16 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -1328,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>0</v>
@@ -1340,16 +1345,16 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
@@ -1358,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>1</v>
@@ -1370,16 +1375,16 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -1388,7 +1393,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>1</v>
@@ -1403,13 +1408,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
@@ -1418,10 +1423,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1430,16 +1435,16 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -1448,10 +1453,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1460,16 +1465,16 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1478,10 +1483,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1490,16 +1495,16 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1508,10 +1513,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1520,16 +1525,16 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -1538,10 +1543,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1550,16 +1555,16 @@
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -1568,10 +1573,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1580,16 +1585,16 @@
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E13" s="5">
         <v>1</v>
@@ -1598,10 +1603,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1610,16 +1615,16 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -1628,10 +1633,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1640,16 +1645,16 @@
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
@@ -1658,10 +1663,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1670,16 +1675,16 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
@@ -1688,10 +1693,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1700,16 +1705,16 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
@@ -1718,10 +1723,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1730,16 +1735,16 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1748,10 +1753,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1760,16 +1765,16 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
@@ -1778,10 +1783,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1790,16 +1795,16 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
@@ -1808,10 +1813,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1820,16 +1825,16 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -1838,10 +1843,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1850,16 +1855,16 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -1868,10 +1873,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1880,16 +1885,16 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
@@ -1898,10 +1903,10 @@
         <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1910,16 +1915,16 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -1928,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1940,16 +1945,16 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -1958,10 +1963,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1970,16 +1975,16 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
@@ -1988,10 +1993,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2000,16 +2005,16 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
@@ -2018,10 +2023,10 @@
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2030,16 +2035,16 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
@@ -2048,10 +2053,10 @@
         <v>0</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2060,16 +2065,16 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E29" s="5">
         <v>1</v>
@@ -2078,10 +2083,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2090,16 +2095,16 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
@@ -2108,10 +2113,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2120,16 +2125,16 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
@@ -2138,10 +2143,10 @@
         <v>0</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2150,16 +2155,16 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
@@ -2168,10 +2173,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2180,16 +2185,16 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
@@ -2198,10 +2203,10 @@
         <v>0</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -2210,16 +2215,16 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
@@ -2228,10 +2233,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -2240,16 +2245,16 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E35" s="5">
         <v>1</v>
@@ -2258,10 +2263,10 @@
         <v>0</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -2270,16 +2275,16 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
@@ -2288,10 +2293,10 @@
         <v>0</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -2300,16 +2305,16 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E37" s="5">
         <v>1</v>
@@ -2318,10 +2323,10 @@
         <v>0</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2330,16 +2335,16 @@
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E38" s="5">
         <v>1</v>
@@ -2348,10 +2353,10 @@
         <v>0</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -2360,16 +2365,16 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E39" s="5">
         <v>1</v>
@@ -2378,10 +2383,10 @@
         <v>0</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -2390,16 +2395,16 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E40" s="5">
         <v>1</v>
@@ -2408,10 +2413,10 @@
         <v>0</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2420,16 +2425,16 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E41" s="5">
         <v>1</v>
@@ -2438,10 +2443,10 @@
         <v>0</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2450,16 +2455,16 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E42" s="5">
         <v>1</v>
@@ -2468,10 +2473,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -2480,16 +2485,16 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E43" s="5">
         <v>1</v>
@@ -2498,10 +2503,10 @@
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -2510,16 +2515,16 @@
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E44" s="5">
         <v>1</v>
@@ -2528,10 +2533,10 @@
         <v>0</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -2540,16 +2545,16 @@
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E45" s="5">
         <v>1</v>
@@ -2558,10 +2563,10 @@
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2570,16 +2575,16 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E46" s="5">
         <v>1</v>
@@ -2588,10 +2593,10 @@
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -2600,16 +2605,16 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E47" s="5">
         <v>1</v>
@@ -2618,10 +2623,10 @@
         <v>0</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2630,16 +2635,16 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E48" s="5">
         <v>1</v>
@@ -2648,10 +2653,10 @@
         <v>0</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2660,16 +2665,16 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E49" s="5">
         <v>1</v>
@@ -2678,10 +2683,10 @@
         <v>0</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2690,16 +2695,16 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E50" s="5">
         <v>1</v>
@@ -2708,10 +2713,10 @@
         <v>0</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2720,16 +2725,16 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E51" s="5">
         <v>1</v>
@@ -2738,10 +2743,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2750,16 +2755,16 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
@@ -2768,10 +2773,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2780,16 +2785,16 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E53" s="5">
         <v>1</v>
@@ -2798,10 +2803,10 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2810,16 +2815,16 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1">
       <c r="A54" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E54" s="5">
         <v>1</v>
@@ -2828,10 +2833,10 @@
         <v>0</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -2840,16 +2845,16 @@
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E55" s="5">
         <v>1</v>
@@ -2858,10 +2863,10 @@
         <v>0</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -2870,16 +2875,16 @@
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
@@ -2888,10 +2893,10 @@
         <v>0</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -2900,16 +2905,16 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E57" s="5">
         <v>1</v>
@@ -2918,10 +2923,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -2930,16 +2935,16 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1">
       <c r="A58" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E58" s="5">
         <v>1</v>
@@ -2948,10 +2953,10 @@
         <v>0</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -2960,16 +2965,16 @@
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E59" s="5">
         <v>1</v>
@@ -2978,10 +2983,10 @@
         <v>0</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -2990,16 +2995,16 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1">
       <c r="A60" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E60" s="5">
         <v>1</v>
@@ -3008,10 +3013,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -3020,16 +3025,16 @@
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
@@ -3038,10 +3043,10 @@
         <v>0</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -3050,16 +3055,16 @@
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E62" s="5">
         <v>1</v>
@@ -3068,10 +3073,10 @@
         <v>0</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -3080,16 +3085,16 @@
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1">
       <c r="A63" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E63" s="5">
         <v>1</v>
@@ -3098,10 +3103,10 @@
         <v>0</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -11657,6 +11662,7 @@
       <c r="L997" s="2"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
re-arrange migrations in preparation for situational dashboard
</commit_message>
<xml_diff>
--- a/SituationalDashboard.xlsx
+++ b/SituationalDashboard.xlsx
@@ -995,12 +995,12 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="25.33203125" customWidth="1"/>
     <col min="5" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
@@ -1060,7 +1060,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>175</v>
@@ -1083,7 +1083,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>175</v>
@@ -1106,7 +1106,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>43</v>
@@ -1152,7 +1152,7 @@
         <v>49</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
more changes to migration
</commit_message>
<xml_diff>
--- a/SituationalDashboard.xlsx
+++ b/SituationalDashboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chart_index" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,391 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="172">
+  <si>
+    <t>t7</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target.Population</t>
+  </si>
+  <si>
+    <t>Number.Missed.Recorded.3days</t>
+  </si>
+  <si>
+    <t>Number.Recovered.3days</t>
+  </si>
+  <si>
+    <t>Percent.Vaccinated.Recorded.3days</t>
+  </si>
+  <si>
+    <t>Percent.Missed.Recorded.3days</t>
+  </si>
+  <si>
+    <t>Number.Recovered.5thDay</t>
+  </si>
+  <si>
+    <t>Total.Recovered</t>
+  </si>
+  <si>
+    <t>Number.Missed.Remain</t>
+  </si>
+  <si>
+    <t>Percent.Missed.Remain</t>
+  </si>
+  <si>
+    <t>Percent.Vaccinated.5days</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t8</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent of FLWs (social mobilisers) paid last campaign</t>
+  </si>
+  <si>
+    <t>Percent FLWs (operation) paid</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent FLWs (operation) paid last campaign</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>District review and planning meeting</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Supervision and monitoring plan updated</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Social mobilisation plan in place</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Social mobilisation plan</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>District governor multi-sectoral meeting</t>
+  </si>
+  <si>
+    <t>Number.Children.Seen.Market.Survey</t>
+  </si>
+  <si>
+    <t>Percent.Coverage.Market.Survey</t>
+  </si>
+  <si>
+    <t>Number.Children.withFM.PCA</t>
+  </si>
+  <si>
+    <t>Number.Children.SeenPCA</t>
+  </si>
+  <si>
+    <t>Percent.Coverage.PCA</t>
+  </si>
+  <si>
+    <t>t9</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t10</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># children seen - PCA</t>
+  </si>
+  <si>
+    <t># children missed due to refusal - PCA</t>
+  </si>
+  <si>
+    <t># children missed due to not available - PCA</t>
+  </si>
+  <si>
+    <t># children missed due to no team visit - PCA</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Immunity Profile</t>
+  </si>
+  <si>
+    <t>100% Stacked Bar</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>Non Polio AFP Rate &amp; Adequate Specimens</t>
+  </si>
+  <si>
+    <t>Bar / Line</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>Innaccessable Children</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>campaign</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>Environmental Results</t>
+  </si>
+  <si>
+    <t>100% Stacked bar</t>
+  </si>
+  <si>
+    <t>t7</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>Campaign Analysis</t>
+  </si>
+  <si>
+    <t>t9</t>
+  </si>
+  <si>
+    <t>Campaign Analysis - Pie Chart</t>
+  </si>
+  <si>
+    <t>Pie Chart</t>
+  </si>
+  <si>
+    <t>t10</t>
+  </si>
+  <si>
+    <t>Missed Children Trend</t>
+  </si>
+  <si>
+    <t>Grouped Bar</t>
+  </si>
+  <si>
+    <t>t11</t>
+  </si>
+  <si>
+    <t>Number Inaccessible Children</t>
+  </si>
+  <si>
+    <t>Total target children</t>
+  </si>
+  <si>
+    <t>Last polio case</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Infected district (Yes/No)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Infected Province (Yes/No)</t>
+  </si>
+  <si>
+    <t>Number of WPV cases</t>
+  </si>
+  <si>
+    <t>data_level</t>
+  </si>
+  <si>
+    <t>date_key</t>
+  </si>
+  <si>
+    <t>month_trend_count</t>
+  </si>
+  <si>
+    <t>t0</t>
+  </si>
+  <si>
+    <t>Basic Banner</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>m_1</t>
+  </si>
+  <si>
+    <t>Polio Cases 2014-Present</t>
+  </si>
+  <si>
+    <t>to_ingest</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>short_name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>data_format</t>
+  </si>
+  <si>
+    <t>good_bound</t>
+  </si>
+  <si>
+    <t>bad_bound</t>
+  </si>
+  <si>
+    <t>source_name</t>
+  </si>
+  <si>
+    <t>chart_key</t>
+  </si>
+  <si>
+    <t>fake</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>chart_type</t>
+  </si>
+  <si>
+    <t>chart</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>fake</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t4</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of Adequate Specimen </t>
+  </si>
+  <si>
+    <t>fake</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t6</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Environmental Samples collected</t>
+  </si>
+  <si>
+    <t>Missed Chilren By Reason</t>
+  </si>
+  <si>
+    <t>Stacked and Grouped Bar</t>
+  </si>
+  <si>
+    <t>t12</t>
+  </si>
+  <si>
+    <t>LQAS</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Number of reported Non Polio AFP cases</t>
+  </si>
+  <si>
+    <t>Number of Unvaccinated Non Polio AFP Cases</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 1-3 doses</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 4-6 doses</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 7+ doses</t>
+  </si>
+  <si>
+    <t>Non Polio AFP Rate</t>
+  </si>
+  <si>
+    <t>SIA service providers identified</t>
+  </si>
+  <si>
+    <t>Percent FLW_operation paid</t>
+  </si>
+  <si>
+    <t>Missed Children PCA vs. Out Of House</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of children missed due to all access issues</t>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent FLW_social mobilisers paid</t>
+  </si>
+  <si>
+    <t>IEC materials displayed</t>
+  </si>
+  <si>
+    <t>Percent volunteers attended training sessions</t>
+  </si>
+  <si>
+    <t>Adequate vaccine arrived</t>
+  </si>
   <si>
     <t>Number of Environmental Samples with Negative result</t>
   </si>
@@ -90,18 +474,10 @@
     <t>Perccent of children who are unvaccinated in the outside monitoring sample</t>
   </si>
   <si>
-    <t>pct</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>fake</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>pct</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>% Missed Children - PCA</t>
   </si>
   <si>
@@ -154,14 +530,6 @@
     <t>Percent children missed due to other reasons - PCA</t>
   </si>
   <si>
-    <t>pct</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>pct</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>t11</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -215,398 +583,6 @@
   </si>
   <si>
     <t>t3</t>
-  </si>
-  <si>
-    <t>Immunity Profile</t>
-  </si>
-  <si>
-    <t>100% Stacked Bar</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>t4</t>
-  </si>
-  <si>
-    <t>Non Polio AFP Rate &amp; Adequate Specimens</t>
-  </si>
-  <si>
-    <t>Bar / Line</t>
-  </si>
-  <si>
-    <t>t5</t>
-  </si>
-  <si>
-    <t>Innaccessable Children</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>campaign</t>
-  </si>
-  <si>
-    <t>t6</t>
-  </si>
-  <si>
-    <t>Environmental Results</t>
-  </si>
-  <si>
-    <t>100% Stacked bar</t>
-  </si>
-  <si>
-    <t>t7</t>
-  </si>
-  <si>
-    <t>t8</t>
-  </si>
-  <si>
-    <t>Campaign Analysis</t>
-  </si>
-  <si>
-    <t>t9</t>
-  </si>
-  <si>
-    <t>Campaign Analysis - Pie Chart</t>
-  </si>
-  <si>
-    <t>Pie Chart</t>
-  </si>
-  <si>
-    <t>t10</t>
-  </si>
-  <si>
-    <t>Missed Children Trend</t>
-  </si>
-  <si>
-    <t>Grouped Bar</t>
-  </si>
-  <si>
-    <t>t11</t>
-  </si>
-  <si>
-    <t>Number Inaccessible Children</t>
-  </si>
-  <si>
-    <t>Total target children</t>
-  </si>
-  <si>
-    <t>Last polio case</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>class</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t0</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Infected district (Yes/No)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Infected Province (Yes/No)</t>
-  </si>
-  <si>
-    <t>Number of WPV cases</t>
-  </si>
-  <si>
-    <t>data_level</t>
-  </si>
-  <si>
-    <t>date_key</t>
-  </si>
-  <si>
-    <t>month_trend_count</t>
-  </si>
-  <si>
-    <t>t0</t>
-  </si>
-  <si>
-    <t>Basic Banner</t>
-  </si>
-  <si>
-    <t>Banner</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>m_1</t>
-  </si>
-  <si>
-    <t>Polio Cases 2014-Present</t>
-  </si>
-  <si>
-    <t>to_ingest</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>short_name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>data_format</t>
-  </si>
-  <si>
-    <t>good_bound</t>
-  </si>
-  <si>
-    <t>bad_bound</t>
-  </si>
-  <si>
-    <t>source_name</t>
-  </si>
-  <si>
-    <t>chart_key</t>
-  </si>
-  <si>
-    <t>fake</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>chart_type</t>
-  </si>
-  <si>
-    <t>chart</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>fake</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t4</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of Adequate Specimen </t>
-  </si>
-  <si>
-    <t>pct</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>fake</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t6</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of Environmental Samples collected</t>
-  </si>
-  <si>
-    <t>Missed Chilren By Reason</t>
-  </si>
-  <si>
-    <t>Stacked and Grouped Bar</t>
-  </si>
-  <si>
-    <t>t12</t>
-  </si>
-  <si>
-    <t>LQAS</t>
-  </si>
-  <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>Number of reported Non Polio AFP cases</t>
-  </si>
-  <si>
-    <t>Number of Unvaccinated Non Polio AFP Cases</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 1-3 doses</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 4-6 doses</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 7+ doses</t>
-  </si>
-  <si>
-    <t>Non Polio AFP Rate</t>
-  </si>
-  <si>
-    <t>SIA service providers identified</t>
-  </si>
-  <si>
-    <t>Percent FLW_operation paid</t>
-  </si>
-  <si>
-    <t>Missed Children PCA vs. Out Of House</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of children missed due to all access issues</t>
-  </si>
-  <si>
-    <t>District</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>District</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent FLW_social mobilisers paid</t>
-  </si>
-  <si>
-    <t>IEC materials displayed</t>
-  </si>
-  <si>
-    <t>Percent volunteers attended training sessions</t>
-  </si>
-  <si>
-    <t>Adequate vaccine arrived</t>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t7</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Target.Population</t>
-  </si>
-  <si>
-    <t>Number.Missed.Recorded.3days</t>
-  </si>
-  <si>
-    <t>Number.Recovered.3days</t>
-  </si>
-  <si>
-    <t>Percent.Vaccinated.Recorded.3days</t>
-  </si>
-  <si>
-    <t>Percent.Missed.Recorded.3days</t>
-  </si>
-  <si>
-    <t>Number.Recovered.5thDay</t>
-  </si>
-  <si>
-    <t>Total.Recovered</t>
-  </si>
-  <si>
-    <t>Number.Missed.Remain</t>
-  </si>
-  <si>
-    <t>Percent.Missed.Remain</t>
-  </si>
-  <si>
-    <t>Percent.Vaccinated.5days</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>pct</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t8</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent of FLWs (social mobilisers) paid last campaign</t>
-  </si>
-  <si>
-    <t>Percent FLWs (operation) paid</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent FLWs (operation) paid last campaign</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>District review and planning meeting</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Supervision and monitoring plan updated</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Social mobilisation plan in place</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Social mobilisation plan</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>District governor multi-sectoral meeting</t>
-  </si>
-  <si>
-    <t>Number.Children.Seen.Market.Survey</t>
-  </si>
-  <si>
-    <t>Percent.Coverage.Market.Survey</t>
-  </si>
-  <si>
-    <t>Number.Children.withFM.PCA</t>
-  </si>
-  <si>
-    <t>Number.Children.SeenPCA</t>
-  </si>
-  <si>
-    <t>Percent.Coverage.PCA</t>
-  </si>
-  <si>
-    <t>t9</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t10</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># children seen - PCA</t>
-  </si>
-  <si>
-    <t># children missed due to refusal - PCA</t>
-  </si>
-  <si>
-    <t># children missed due to not available - PCA</t>
-  </si>
-  <si>
-    <t># children missed due to no team visit - PCA</t>
   </si>
 </sst>
 </file>
@@ -984,7 +960,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -995,7 +971,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1009,62 +985,62 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>167</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G3" s="1">
         <v>28</v>
@@ -1072,22 +1048,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>170</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1">
         <v>28</v>
@@ -1095,22 +1071,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1">
         <v>28</v>
@@ -1118,22 +1094,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1">
         <v>16</v>
@@ -1141,22 +1117,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1">
         <v>3</v>
@@ -1164,22 +1140,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G8" s="1">
         <v>28</v>
@@ -1187,22 +1163,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>144</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>170</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G9" s="1">
         <v>3</v>
@@ -1210,22 +1186,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>170</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
@@ -1233,22 +1209,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1256,22 +1232,22 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G12" s="1">
         <v>3</v>
@@ -1279,22 +1255,22 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G13" s="1">
         <v>3</v>
@@ -1302,22 +1278,22 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G14" s="1">
         <v>3</v>
@@ -1325,29 +1301,28 @@
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>133</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G15" s="1">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1363,8 +1338,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L997"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
@@ -1384,28 +1359,28 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1413,16 +1388,16 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -1431,10 +1406,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1442,16 +1417,16 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -1460,10 +1435,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1472,16 +1447,16 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -1490,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1502,16 +1477,16 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
@@ -1520,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1532,16 +1507,16 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -1550,10 +1525,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1562,16 +1537,16 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
@@ -1580,10 +1555,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1592,16 +1567,16 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -1610,10 +1585,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1622,16 +1597,16 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1640,10 +1615,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1652,16 +1627,16 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1670,10 +1645,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1682,16 +1657,16 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -1700,10 +1675,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1712,16 +1687,16 @@
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -1730,10 +1705,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1742,16 +1717,16 @@
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="E13" s="10">
         <v>1</v>
@@ -1760,10 +1735,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1772,16 +1747,16 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -1790,10 +1765,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1802,16 +1777,16 @@
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
@@ -1820,10 +1795,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1832,16 +1807,16 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
@@ -1850,10 +1825,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1862,16 +1837,16 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
@@ -1880,10 +1855,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1892,16 +1867,16 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>121</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1910,10 +1885,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1922,16 +1897,16 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>162</v>
+        <v>16</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>143</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
@@ -1940,10 +1915,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1952,16 +1927,16 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>4</v>
+        <v>123</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
@@ -1970,10 +1945,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1982,16 +1957,16 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
+        <v>145</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -2000,10 +1975,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2012,16 +1987,16 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>163</v>
+        <v>17</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -2030,10 +2005,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2042,16 +2017,16 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>164</v>
+        <v>18</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>165</v>
+        <v>19</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
@@ -2060,10 +2035,10 @@
         <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2072,16 +2047,16 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>166</v>
+        <v>20</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>8</v>
+        <v>127</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -2090,10 +2065,10 @@
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2102,16 +2077,16 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -2120,10 +2095,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2132,16 +2107,16 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
@@ -2150,10 +2125,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2162,16 +2137,16 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>159</v>
+        <v>13</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
@@ -2180,10 +2155,10 @@
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2192,16 +2167,16 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
@@ -2210,10 +2185,10 @@
         <v>0</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2222,16 +2197,16 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>115</v>
+        <v>33</v>
       </c>
       <c r="E29" s="5">
         <v>1</v>
@@ -2240,10 +2215,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2252,16 +2227,16 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>50</v>
+        <v>165</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
@@ -2270,10 +2245,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2282,16 +2257,16 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
@@ -2300,10 +2275,10 @@
         <v>0</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2312,16 +2287,16 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
@@ -2330,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2342,16 +2317,16 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>147</v>
+        <v>2</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>147</v>
+        <v>2</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>147</v>
+        <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
@@ -2360,10 +2335,10 @@
         <v>0</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -2372,16 +2347,16 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
@@ -2390,10 +2365,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -2402,16 +2377,16 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E35" s="5">
         <v>1</v>
@@ -2420,10 +2395,10 @@
         <v>0</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -2432,16 +2407,16 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
@@ -2450,10 +2425,10 @@
         <v>0</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -2462,16 +2437,16 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>151</v>
+        <v>6</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>151</v>
+        <v>6</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>151</v>
+        <v>6</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E37" s="5">
         <v>1</v>
@@ -2480,10 +2455,10 @@
         <v>0</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2492,16 +2467,16 @@
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E38" s="5">
         <v>1</v>
@@ -2510,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -2522,16 +2497,16 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>153</v>
+        <v>8</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>153</v>
+        <v>8</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>153</v>
+        <v>8</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E39" s="5">
         <v>1</v>
@@ -2540,10 +2515,10 @@
         <v>0</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -2552,16 +2527,16 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>157</v>
+        <v>60</v>
       </c>
       <c r="E40" s="5">
         <v>1</v>
@@ -2570,10 +2545,10 @@
         <v>0</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2582,16 +2557,16 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E41" s="5">
         <v>1</v>
@@ -2600,10 +2575,10 @@
         <v>0</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2612,16 +2587,16 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E42" s="5">
         <v>1</v>
@@ -2630,10 +2605,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -2642,16 +2617,16 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E43" s="5">
         <v>1</v>
@@ -2660,10 +2635,10 @@
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -2672,16 +2647,16 @@
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>167</v>
+        <v>21</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>167</v>
+        <v>21</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>167</v>
+        <v>21</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E44" s="5">
         <v>1</v>
@@ -2690,10 +2665,10 @@
         <v>0</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -2702,16 +2677,16 @@
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E45" s="5">
         <v>1</v>
@@ -2720,10 +2695,10 @@
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2732,16 +2707,16 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E46" s="5">
         <v>1</v>
@@ -2750,10 +2725,10 @@
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -2762,16 +2737,16 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>170</v>
+        <v>24</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>170</v>
+        <v>24</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>170</v>
+        <v>24</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E47" s="5">
         <v>1</v>
@@ -2780,10 +2755,10 @@
         <v>0</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2792,16 +2767,16 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>171</v>
+        <v>25</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>171</v>
+        <v>25</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>171</v>
+        <v>25</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E48" s="5">
         <v>1</v>
@@ -2810,10 +2785,10 @@
         <v>0</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2822,16 +2797,16 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E49" s="5">
         <v>1</v>
@@ -2840,10 +2815,10 @@
         <v>0</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>173</v>
+        <v>27</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2852,16 +2827,16 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="E50" s="5">
         <v>1</v>
@@ -2870,10 +2845,10 @@
         <v>0</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>173</v>
+        <v>27</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2882,16 +2857,16 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E51" s="5">
         <v>1</v>
@@ -2900,10 +2875,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>173</v>
+        <v>27</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2912,16 +2887,16 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>174</v>
+        <v>28</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>174</v>
+        <v>28</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
@@ -2930,10 +2905,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2942,16 +2917,16 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E53" s="5">
         <v>1</v>
@@ -2960,10 +2935,10 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2972,16 +2947,16 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1">
       <c r="A54" s="9" t="s">
-        <v>176</v>
+        <v>30</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>176</v>
+        <v>30</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>176</v>
+        <v>30</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E54" s="5">
         <v>1</v>
@@ -2990,10 +2965,10 @@
         <v>0</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -3002,16 +2977,16 @@
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E55" s="5">
         <v>1</v>
@@ -3020,10 +2995,10 @@
         <v>0</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -3032,16 +3007,16 @@
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
@@ -3050,10 +3025,10 @@
         <v>0</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -3062,16 +3037,16 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E57" s="5">
         <v>1</v>
@@ -3080,10 +3055,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -3092,16 +3067,16 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1">
       <c r="A58" s="9" t="s">
-        <v>36</v>
+        <v>153</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>36</v>
+        <v>153</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>36</v>
+        <v>153</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E58" s="5">
         <v>1</v>
@@ -3110,10 +3085,10 @@
         <v>0</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -3122,16 +3097,16 @@
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E59" s="5">
         <v>1</v>
@@ -3140,10 +3115,10 @@
         <v>0</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -3152,16 +3127,16 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1">
       <c r="A60" s="9" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E60" s="5">
         <v>1</v>
@@ -3170,10 +3145,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -3182,16 +3157,16 @@
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
@@ -3200,10 +3175,10 @@
         <v>0</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -3212,16 +3187,16 @@
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E62" s="5">
         <v>1</v>
@@ -3230,10 +3205,10 @@
         <v>0</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -3242,16 +3217,16 @@
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1">
       <c r="A63" s="8" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E63" s="5">
         <v>1</v>
@@ -3260,10 +3235,10 @@
         <v>0</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -3272,16 +3247,16 @@
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1">
       <c r="A64" s="5" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E64" s="5">
         <v>1</v>
@@ -3290,10 +3265,10 @@
         <v>0</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
@@ -3302,16 +3277,16 @@
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1">
       <c r="A65" s="5" t="s">
-        <v>23</v>
+        <v>140</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>23</v>
+        <v>140</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E65" s="5">
         <v>1</v>
@@ -3320,10 +3295,10 @@
         <v>0</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
@@ -3332,16 +3307,16 @@
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1">
       <c r="A66" s="5" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>26</v>
+        <v>143</v>
       </c>
       <c r="E66" s="5">
         <v>1</v>
@@ -3350,10 +3325,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
@@ -11867,9 +11842,9 @@
       <c r="L997" s="2"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
fixed most of migrations
</commit_message>
<xml_diff>
--- a/SituationalDashboard.xlsx
+++ b/SituationalDashboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19840" windowHeight="16420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chart_index" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,360 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="167">
+  <si>
+    <t>Supervision and Monitoring Plan</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t13</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t13</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stacked Column Chart</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>campaign</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Perccent of children who are unvaccinated in the outside monitoring sample</t>
+  </si>
+  <si>
+    <t>fake</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent missed children</t>
+  </si>
+  <si>
+    <t>polio cases</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Preparatory Indicators</t>
+  </si>
+  <si>
+    <t>Percent FLWs (social mobilisers) paid</t>
+  </si>
+  <si>
+    <t># children missed due to other reasons - PCA</t>
+  </si>
+  <si>
+    <t>Percent children missed due to refusal - PCA</t>
+  </si>
+  <si>
+    <t>Percent children missed due to not available - PCA</t>
+  </si>
+  <si>
+    <t>Percent children missed due to no team visit - PCA</t>
+  </si>
+  <si>
+    <t>Percent children missed due to other reasons - PCA</t>
+  </si>
+  <si>
+    <t>t11</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># of Accepted Lots by 90%</t>
+  </si>
+  <si>
+    <t># of Accepted Lots by 80%</t>
+  </si>
+  <si>
+    <t># of Rejected Lots by 80%</t>
+  </si>
+  <si>
+    <t>t12</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent volunteers trained</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent of volunteers attended training sessions</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bubble Map</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>Annual Case Table</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>IEC Materials Displayed</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Microplan Reviewed and Updated</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Microplan Reviewed and Updated</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>District Review and Planning Meeting</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLW Training Plan Updated</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adequate Vaccine Arrived</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>District Governor Multi-Sectoral Meeting</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIA service providers</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Social Mobilisation Plan</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Infected district (Yes/No)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Infected Province (Yes/No)</t>
+  </si>
+  <si>
+    <t>Number of WPV cases</t>
+  </si>
+  <si>
+    <t>data_level</t>
+  </si>
+  <si>
+    <t>date_key</t>
+  </si>
+  <si>
+    <t>month_trend_count</t>
+  </si>
+  <si>
+    <t>t0</t>
+  </si>
+  <si>
+    <t>Basic Banner</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>m_1</t>
+  </si>
+  <si>
+    <t>Polio Cases 2014-Present</t>
+  </si>
+  <si>
+    <t>to_ingest</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>short_name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>data_format</t>
+  </si>
+  <si>
+    <t>good_bound</t>
+  </si>
+  <si>
+    <t>bad_bound</t>
+  </si>
+  <si>
+    <t>source_name</t>
+  </si>
+  <si>
+    <t>chart_key</t>
+  </si>
+  <si>
+    <t>fake</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>chart_type</t>
+  </si>
+  <si>
+    <t>chart</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>fake</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t4</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of Adequate Specimen </t>
+  </si>
+  <si>
+    <t>fake</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t6</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Environmental Samples collected</t>
+  </si>
+  <si>
+    <t>Missed Chilren By Reason</t>
+  </si>
+  <si>
+    <t>Stacked and Grouped Bar</t>
+  </si>
+  <si>
+    <t>t12</t>
+  </si>
+  <si>
+    <t>LQAS</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Number of reported Non Polio AFP cases</t>
+  </si>
+  <si>
+    <t>Number of Unvaccinated Non Polio AFP Cases</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 1-3 doses</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 4-6 doses</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 7+ doses</t>
+  </si>
+  <si>
+    <t>Non Polio AFP Rate</t>
+  </si>
+  <si>
+    <t>SIA service providers identified</t>
+  </si>
+  <si>
+    <t>Percent FLW_operation paid</t>
+  </si>
+  <si>
+    <t>Missed Children PCA vs. Out Of House</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of children missed due to all access issues</t>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent FLW_social mobilisers paid</t>
+  </si>
+  <si>
+    <t>Percent volunteers attended training sessions</t>
+  </si>
+  <si>
+    <t>Number of Environmental Samples with Negative result</t>
+  </si>
+  <si>
+    <t>Number of Environmental Samples with Positive result</t>
+  </si>
+  <si>
+    <t>Number of Environmental Samples with result pending in Lab</t>
+  </si>
+  <si>
+    <t>Supervision and monitoring plan</t>
+  </si>
+  <si>
+    <t>Social mobilization plan</t>
+  </si>
+  <si>
+    <t>District Governor multi-sectoral meeting on Polio</t>
+  </si>
+  <si>
+    <t>Number.Vaccinated.Recorded.3days</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>fake</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number.Children.withFM.Market.Survey</t>
+  </si>
+  <si>
+    <t># children seen - PCA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
   <si>
     <t>t7</t>
     <phoneticPr fontId="9" type="noConversion"/>
@@ -75,25 +428,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>District review and planning meeting</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Supervision and monitoring plan updated</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Social mobilisation plan in place</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Social mobilisation plan</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>District governor multi-sectoral meeting</t>
-  </si>
-  <si>
     <t>Number.Children.Seen.Market.Survey</t>
   </si>
   <si>
@@ -137,6 +471,30 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
+    <t>Number of Environmental Samples collected</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of Adequate Specimen </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Environmental Samples with Negative result</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent Missed Children - Out of House Survey</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent Missed Children - Out of House Survey</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent Missed Children - PCA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
     <t>Immunity Profile</t>
   </si>
   <si>
@@ -217,372 +575,6 @@
   <si>
     <t>int</t>
     <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>class</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t0</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Infected district (Yes/No)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Infected Province (Yes/No)</t>
-  </si>
-  <si>
-    <t>Number of WPV cases</t>
-  </si>
-  <si>
-    <t>data_level</t>
-  </si>
-  <si>
-    <t>date_key</t>
-  </si>
-  <si>
-    <t>month_trend_count</t>
-  </si>
-  <si>
-    <t>t0</t>
-  </si>
-  <si>
-    <t>Basic Banner</t>
-  </si>
-  <si>
-    <t>Banner</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>m_1</t>
-  </si>
-  <si>
-    <t>Polio Cases 2014-Present</t>
-  </si>
-  <si>
-    <t>to_ingest</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>short_name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>data_format</t>
-  </si>
-  <si>
-    <t>good_bound</t>
-  </si>
-  <si>
-    <t>bad_bound</t>
-  </si>
-  <si>
-    <t>source_name</t>
-  </si>
-  <si>
-    <t>chart_key</t>
-  </si>
-  <si>
-    <t>fake</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>chart_type</t>
-  </si>
-  <si>
-    <t>chart</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>fake</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t4</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of Adequate Specimen </t>
-  </si>
-  <si>
-    <t>fake</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t6</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of Environmental Samples collected</t>
-  </si>
-  <si>
-    <t>Missed Chilren By Reason</t>
-  </si>
-  <si>
-    <t>Stacked and Grouped Bar</t>
-  </si>
-  <si>
-    <t>t12</t>
-  </si>
-  <si>
-    <t>LQAS</t>
-  </si>
-  <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>Number of reported Non Polio AFP cases</t>
-  </si>
-  <si>
-    <t>Number of Unvaccinated Non Polio AFP Cases</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 1-3 doses</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 4-6 doses</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 7+ doses</t>
-  </si>
-  <si>
-    <t>Non Polio AFP Rate</t>
-  </si>
-  <si>
-    <t>SIA service providers identified</t>
-  </si>
-  <si>
-    <t>Percent FLW_operation paid</t>
-  </si>
-  <si>
-    <t>Missed Children PCA vs. Out Of House</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of children missed due to all access issues</t>
-  </si>
-  <si>
-    <t>District</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>District</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent FLW_social mobilisers paid</t>
-  </si>
-  <si>
-    <t>IEC materials displayed</t>
-  </si>
-  <si>
-    <t>Percent volunteers attended training sessions</t>
-  </si>
-  <si>
-    <t>Adequate vaccine arrived</t>
-  </si>
-  <si>
-    <t>Number of Environmental Samples with Negative result</t>
-  </si>
-  <si>
-    <t>Number of Environmental Samples with Positive result</t>
-  </si>
-  <si>
-    <t>Number of Environmental Samples with result pending in Lab</t>
-  </si>
-  <si>
-    <t>District review and planning meeting</t>
-  </si>
-  <si>
-    <t>Micro-plan reviewed_updated</t>
-  </si>
-  <si>
-    <t>FLWs training plan</t>
-  </si>
-  <si>
-    <t>Supervision and monitoring plan</t>
-  </si>
-  <si>
-    <t>Social mobilization plan</t>
-  </si>
-  <si>
-    <t>District Governor multi-sectoral meeting on Polio</t>
-  </si>
-  <si>
-    <t>Number.Vaccinated.Recorded.3days</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>fake</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number.Children.withFM.Market.Survey</t>
-  </si>
-  <si>
-    <t># children seen - PCA</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t13</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t13</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>District</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stacked Column Chart</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>campaign</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>% Missed Children - Out of House Survey</t>
-  </si>
-  <si>
-    <t>Perccent of children who are unvaccinated in the outside monitoring sample</t>
-  </si>
-  <si>
-    <t>fake</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>% Missed Children - PCA</t>
-  </si>
-  <si>
-    <t>Percent missed children</t>
-  </si>
-  <si>
-    <t>polio cases</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Preparatory Indicators</t>
-  </si>
-  <si>
-    <t>FLW training plan</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Microplan review_update</t>
-  </si>
-  <si>
-    <t>Microplan reviewed and updated</t>
-  </si>
-  <si>
-    <t>SIA Service Providers</t>
-  </si>
-  <si>
-    <t>SIA service providers selected</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent FLWs (social mobilisers) paid</t>
-  </si>
-  <si>
-    <t># children missed due to other reasons - PCA</t>
-  </si>
-  <si>
-    <t>Percent children missed due to refusal - PCA</t>
-  </si>
-  <si>
-    <t>Percent children missed due to not available - PCA</t>
-  </si>
-  <si>
-    <t>Percent children missed due to no team visit - PCA</t>
-  </si>
-  <si>
-    <t>Percent children missed due to other reasons - PCA</t>
-  </si>
-  <si>
-    <t>t11</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># of Accepted Lots by 90%</t>
-  </si>
-  <si>
-    <t># of Accepted Lots by 80%</t>
-  </si>
-  <si>
-    <t># of Rejected Lots by 80%</t>
-  </si>
-  <si>
-    <t>t12</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>District Governor multi-sectoral meeting on Polio conducted</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent volunteers trained</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent of volunteers attended training sessions</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adequate vaccine arrived</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adequate vaccine arrived one day before campaign</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>FLW training plan updated</t>
-  </si>
-  <si>
-    <t>Bubble Map</t>
-  </si>
-  <si>
-    <t>t2</t>
-  </si>
-  <si>
-    <t>Annual Case Table</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>t3</t>
   </si>
 </sst>
 </file>
@@ -675,7 +667,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -689,6 +681,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -960,7 +953,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -972,7 +965,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
@@ -985,62 +978,62 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>167</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1">
         <v>28</v>
@@ -1048,22 +1041,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>170</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1">
         <v>28</v>
@@ -1071,22 +1064,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="G5" s="1">
         <v>28</v>
@@ -1094,22 +1087,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1">
         <v>16</v>
@@ -1117,22 +1110,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="G7" s="1">
         <v>3</v>
@@ -1140,22 +1133,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>151</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1">
         <v>28</v>
@@ -1163,22 +1156,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>144</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>170</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="G9" s="1">
         <v>3</v>
@@ -1186,22 +1179,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>170</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
@@ -1209,22 +1202,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1232,22 +1225,22 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>161</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="G12" s="1">
         <v>3</v>
@@ -1255,22 +1248,22 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>162</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="G13" s="1">
         <v>3</v>
@@ -1278,22 +1271,22 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="G14" s="1">
         <v>3</v>
@@ -1301,22 +1294,22 @@
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>133</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>134</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>136</v>
+        <v>5</v>
       </c>
       <c r="G15" s="1">
         <v>28</v>
@@ -1338,8 +1331,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
@@ -1359,28 +1352,28 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1388,16 +1381,16 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -1406,10 +1399,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1417,16 +1410,16 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>59</v>
+        <v>165</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>59</v>
+        <v>165</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>59</v>
+        <v>165</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -1435,10 +1428,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1447,16 +1440,16 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -1465,10 +1458,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1477,16 +1470,16 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
@@ -1495,10 +1488,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1507,16 +1500,16 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -1525,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1537,16 +1530,16 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
@@ -1555,10 +1548,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1567,16 +1560,16 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -1585,10 +1578,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1597,16 +1590,16 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1615,10 +1608,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1627,16 +1620,16 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1645,10 +1638,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1657,16 +1650,16 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -1675,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1687,16 +1680,16 @@
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -1705,10 +1698,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1717,16 +1710,16 @@
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E13" s="10">
         <v>1</v>
@@ -1735,10 +1728,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1747,16 +1740,16 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -1765,10 +1758,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1776,17 +1769,17 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A15" t="s">
-        <v>94</v>
+      <c r="A15" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
@@ -1795,10 +1788,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1806,17 +1799,17 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A16" t="s">
-        <v>119</v>
+      <c r="A16" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
@@ -1825,10 +1818,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1837,16 +1830,16 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
@@ -1855,10 +1848,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1867,16 +1860,16 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1885,10 +1878,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1897,16 +1890,16 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
@@ -1915,10 +1908,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1926,17 +1919,17 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>123</v>
+      <c r="A20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
@@ -1945,10 +1938,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1957,16 +1950,16 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>145</v>
+        <v>34</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -1975,10 +1968,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1987,16 +1980,16 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -2005,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2017,16 +2010,16 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
@@ -2035,10 +2028,10 @@
         <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2047,16 +2040,16 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>161</v>
+        <v>36</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -2065,10 +2058,10 @@
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2077,16 +2070,16 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>149</v>
+        <v>37</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>148</v>
+        <v>37</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -2095,10 +2088,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2107,16 +2100,16 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
@@ -2125,10 +2118,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2137,16 +2130,16 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>150</v>
+        <v>12</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
@@ -2155,10 +2148,10 @@
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2167,16 +2160,16 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
@@ -2185,10 +2178,10 @@
         <v>0</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2197,16 +2190,16 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>163</v>
+        <v>24</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>162</v>
+        <v>23</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="E29" s="5">
         <v>1</v>
@@ -2215,10 +2208,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2227,16 +2220,16 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>165</v>
+        <v>35</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
@@ -2245,10 +2238,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2257,16 +2250,16 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
@@ -2275,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2287,16 +2280,16 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
@@ -2305,10 +2298,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2317,16 +2310,16 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
@@ -2335,10 +2328,10 @@
         <v>0</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -2347,16 +2340,16 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
@@ -2365,10 +2358,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -2377,16 +2370,16 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E35" s="5">
         <v>1</v>
@@ -2395,10 +2388,10 @@
         <v>0</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -2407,16 +2400,16 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
@@ -2425,10 +2418,10 @@
         <v>0</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -2437,16 +2430,16 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E37" s="5">
         <v>1</v>
@@ -2455,10 +2448,10 @@
         <v>0</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2467,16 +2460,16 @@
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E38" s="5">
         <v>1</v>
@@ -2485,10 +2478,10 @@
         <v>0</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -2497,16 +2490,16 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E39" s="5">
         <v>1</v>
@@ -2515,10 +2508,10 @@
         <v>0</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -2527,16 +2520,16 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="E40" s="5">
         <v>1</v>
@@ -2545,10 +2538,10 @@
         <v>0</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2557,16 +2550,16 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E41" s="5">
         <v>1</v>
@@ -2575,10 +2568,10 @@
         <v>0</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2587,16 +2580,16 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E42" s="5">
         <v>1</v>
@@ -2605,10 +2598,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -2617,16 +2610,16 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E43" s="5">
         <v>1</v>
@@ -2635,10 +2628,10 @@
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -2647,16 +2640,16 @@
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E44" s="5">
         <v>1</v>
@@ -2665,10 +2658,10 @@
         <v>0</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -2677,16 +2670,16 @@
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E45" s="5">
         <v>1</v>
@@ -2695,10 +2688,10 @@
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2707,16 +2700,16 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E46" s="5">
         <v>1</v>
@@ -2725,10 +2718,10 @@
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -2737,16 +2730,16 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E47" s="5">
         <v>1</v>
@@ -2755,10 +2748,10 @@
         <v>0</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2767,16 +2760,16 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E48" s="5">
         <v>1</v>
@@ -2785,10 +2778,10 @@
         <v>0</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2797,16 +2790,16 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E49" s="5">
         <v>1</v>
@@ -2815,10 +2808,10 @@
         <v>0</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2827,16 +2820,16 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="E50" s="5">
         <v>1</v>
@@ -2845,10 +2838,10 @@
         <v>0</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2857,16 +2850,16 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E51" s="5">
         <v>1</v>
@@ -2875,10 +2868,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2887,16 +2880,16 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
@@ -2905,10 +2898,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2917,16 +2910,16 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E53" s="5">
         <v>1</v>
@@ -2935,10 +2928,10 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2947,16 +2940,16 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1">
       <c r="A54" s="9" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E54" s="5">
         <v>1</v>
@@ -2965,10 +2958,10 @@
         <v>0</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -2977,16 +2970,16 @@
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E55" s="5">
         <v>1</v>
@@ -2995,10 +2988,10 @@
         <v>0</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -3007,16 +3000,16 @@
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>151</v>
+        <v>13</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>151</v>
+        <v>13</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>151</v>
+        <v>13</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
@@ -3025,10 +3018,10 @@
         <v>0</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -3037,16 +3030,16 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>152</v>
+        <v>14</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>152</v>
+        <v>14</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>152</v>
+        <v>14</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E57" s="5">
         <v>1</v>
@@ -3055,10 +3048,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -3067,16 +3060,16 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1">
       <c r="A58" s="9" t="s">
-        <v>153</v>
+        <v>15</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>153</v>
+        <v>15</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>153</v>
+        <v>15</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E58" s="5">
         <v>1</v>
@@ -3085,10 +3078,10 @@
         <v>0</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -3097,16 +3090,16 @@
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>154</v>
+        <v>16</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>154</v>
+        <v>16</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>154</v>
+        <v>16</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E59" s="5">
         <v>1</v>
@@ -3115,10 +3108,10 @@
         <v>0</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -3127,16 +3120,16 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1">
       <c r="A60" s="9" t="s">
-        <v>155</v>
+        <v>17</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>155</v>
+        <v>17</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>155</v>
+        <v>17</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E60" s="5">
         <v>1</v>
@@ -3145,10 +3138,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -3157,16 +3150,16 @@
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>157</v>
+        <v>19</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>157</v>
+        <v>19</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>157</v>
+        <v>19</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
@@ -3175,10 +3168,10 @@
         <v>0</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -3187,16 +3180,16 @@
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E62" s="5">
         <v>1</v>
@@ -3205,10 +3198,10 @@
         <v>0</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -3217,16 +3210,16 @@
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1">
       <c r="A63" s="8" t="s">
-        <v>159</v>
+        <v>21</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>159</v>
+        <v>21</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>159</v>
+        <v>21</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E63" s="5">
         <v>1</v>
@@ -3235,10 +3228,10 @@
         <v>0</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -3250,13 +3243,13 @@
         <v>137</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>138</v>
+        <v>6</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E64" s="5">
         <v>1</v>
@@ -3265,10 +3258,10 @@
         <v>0</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
@@ -3277,16 +3270,16 @@
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1">
       <c r="A65" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>141</v>
+        <v>8</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="E65" s="5">
         <v>1</v>
@@ -3295,10 +3288,10 @@
         <v>0</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
@@ -3307,16 +3300,16 @@
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1">
       <c r="A66" s="5" t="s">
-        <v>142</v>
+        <v>9</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>142</v>
+        <v>9</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>142</v>
+        <v>9</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="E66" s="5">
         <v>1</v>
@@ -3325,10 +3318,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>

</xml_diff>